<commit_message>
Added the parallel matlab code.
</commit_message>
<xml_diff>
--- a/Results/Weizmann/Accuracy_Analysis_Vocabulary_Size_100_Kernel_Linear.xlsx
+++ b/Results/Weizmann/Accuracy_Analysis_Vocabulary_Size_100_Kernel_Linear.xlsx
@@ -449,10 +449,10 @@
   <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>